<commit_message>
Changes to be committed: 	modified:   Tests.xlsx 	modified:   database/frameworks.json 	modified:   index.html 	modified:   index.js 	modified:   logic/fileHandle.js 	new file:   sprawozdanie_ZDINF.docx
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sieni\OneDrive\Szkoła\Zimowy_2022\Zarządzanie danymi informacyjnymi\2_Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sieni\OneDrive\Szkoła\Zimowy_2022\Podstawy języków Skryptowych\2_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA98263D-A007-4A76-B95B-C8245484069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3ED46D-70D6-4D98-B087-CBCE0AD187FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,6 +52,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,10 +98,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dobry" xfId="1" builtinId="26"/>
@@ -172,60 +176,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:numRef>
@@ -258,25 +209,25 @@
             <c:numRef>
               <c:f>Sheet1!$C$3:$H$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>299999</c:v>
+                  <c:v>0.2158203125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000000</c:v>
+                  <c:v>0.840087890625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3700000</c:v>
+                  <c:v>1.97607421875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3299999</c:v>
+                  <c:v>3.751953125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5500000</c:v>
+                  <c:v>7.2578125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8200000</c:v>
+                  <c:v>12.453125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -313,106 +264,31 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-6.5931495405179619E-2"/>
-                  <c:y val="-1.8583040707345757E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-8EF3-405D-93E1-36BFE7C5B45F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$4:$H$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>200000</c:v>
+                  <c:v>5.615234375E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>99999</c:v>
+                  <c:v>6.103515625E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99999</c:v>
+                  <c:v>0.193115234375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>299999</c:v>
+                  <c:v>8.5693359375E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>600000</c:v>
+                  <c:v>0.10888671875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1100000</c:v>
+                  <c:v>8.6181640625E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -449,84 +325,31 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$5:$H$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.099609375E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.126953125E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99999</c:v>
+                  <c:v>5.126953125E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100000</c:v>
+                  <c:v>4.00390625E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400000</c:v>
+                  <c:v>4.00390625E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>299999</c:v>
+                  <c:v>3.1982421875E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -563,106 +386,31 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.3692564745196446E-2"/>
-                  <c:y val="-3.4068907963467121E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-8EF3-405D-93E1-36BFE7C5B45F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$6:$H$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9.4970703125E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.90625E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>2.19726562E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4.6142578125E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>299999</c:v>
+                  <c:v>7.7880859375E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>299999</c:v>
+                  <c:v>6.2255859375E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -788,7 +536,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -989,66 +737,13 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$12:$H$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
@@ -1075,25 +770,25 @@
             <c:numRef>
               <c:f>Sheet1!$C$13:$H$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>299999</c:v>
+                  <c:v>0.348876953125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1600000</c:v>
+                  <c:v>0.35107421875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000000</c:v>
+                  <c:v>3.35986328125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4599999</c:v>
+                  <c:v>6.52099609375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29099999</c:v>
+                  <c:v>9.080078125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43199999</c:v>
+                  <c:v>15.324951171875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,84 +825,31 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$14:$H$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.4169921875E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.10400390625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.9814453125E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.248046875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.56396484375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100000</c:v>
+                  <c:v>0.794921875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,84 +886,31 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$15:$H$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.197265625E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.0009765625E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.90625E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9.912109375E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.291015625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.35205078125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1358,84 +947,31 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$16:$H$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.293212890625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.787109375E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.0009765625E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.10400390625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.23486328125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.33203125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1492,7 +1028,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1561,7 +1097,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2899,16 +2435,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2935,16 +2471,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3238,18 +2774,23 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
@@ -3279,119 +2820,157 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>299999</v>
-      </c>
-      <c r="D3">
-        <v>1000000</v>
-      </c>
-      <c r="E3">
-        <v>3700000</v>
-      </c>
-      <c r="F3">
-        <v>3299999</v>
-      </c>
-      <c r="G3">
-        <v>5500000</v>
-      </c>
-      <c r="H3">
-        <v>8200000</v>
+      <c r="C3" s="2">
+        <v>0.2158203125</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.840087890625</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.97607421875</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3.751953125</v>
+      </c>
+      <c r="G3" s="2">
+        <v>7.2578125</v>
+      </c>
+      <c r="H3" s="2">
+        <v>12.453125</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>200000</v>
-      </c>
-      <c r="D4">
-        <v>99999</v>
-      </c>
-      <c r="E4">
-        <v>99999</v>
-      </c>
-      <c r="F4">
-        <v>299999</v>
-      </c>
-      <c r="G4">
-        <v>600000</v>
-      </c>
-      <c r="H4">
-        <v>1100000</v>
+      <c r="C4" s="2">
+        <v>5.615234375E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.103515625E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.193115234375</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8.5693359375E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.10888671875</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8.6181640625E-2</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>99999</v>
-      </c>
-      <c r="F5">
-        <v>100000</v>
-      </c>
-      <c r="G5">
-        <v>400000</v>
-      </c>
-      <c r="H5">
-        <v>299999</v>
+      <c r="C5" s="2">
+        <v>2.099609375E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5.126953125E-3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.126953125E-3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4.00390625E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4.00390625E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3.1982421875E-2</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>200000</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>299999</v>
-      </c>
-      <c r="H6">
-        <v>299999</v>
-      </c>
+      <c r="C6" s="2">
+        <v>9.4970703125E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.19726562E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4.6142578125E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>7.7880859375E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>6.2255859375E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>1000</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>10000</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>50000</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>100000</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
         <v>300000</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="3">
         <v>500000</v>
       </c>
     </row>
@@ -3399,92 +2978,92 @@
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
-        <v>299999</v>
-      </c>
-      <c r="D13">
-        <v>1600000</v>
-      </c>
-      <c r="E13">
-        <v>4000000</v>
-      </c>
-      <c r="F13">
-        <v>4599999</v>
-      </c>
-      <c r="G13">
-        <v>29099999</v>
-      </c>
-      <c r="H13">
-        <v>43199999</v>
+      <c r="C13" s="2">
+        <v>0.348876953125</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.35107421875</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3.35986328125</v>
+      </c>
+      <c r="F13" s="2">
+        <v>6.52099609375</v>
+      </c>
+      <c r="G13" s="2">
+        <v>9.080078125</v>
+      </c>
+      <c r="H13" s="2">
+        <v>15.324951171875</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
+      <c r="C14" s="2">
+        <v>2.4169921875E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.10400390625</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5.9814453125E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.248046875</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>100000</v>
+        <v>0.56396484375</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.794921875</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
+      <c r="C15" s="2">
+        <v>2.197265625E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.0009765625E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9.912109375E-2</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
+        <v>0.291015625</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.35205078125</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
+      <c r="C16" s="2">
+        <v>0.293212890625</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6.787109375E-2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.0009765625E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.10400390625</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
+        <v>0.23486328125</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.33203125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>